<commit_message>
FUNCTIONAL for download of xlsx and merge
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,1026 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>MrNumber</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Productlink</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Domain</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Outcome</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>DateOfOutcome</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>UpdatedAt</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MAHolder</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>RMS</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ActiveSubstances</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>AtcCodes</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>CMS</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>DoseForms</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Documents</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>WithdrawalReasons</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Typelevel1</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Typelevel2</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Typelevel3</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Typelevel4</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Typelevel5</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>NL/H/4002/003</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4002/003</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Dasatinib Sandoz 70 mg, filmomhulde tabletten</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2018-07-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2023-01-20T11:02:17.337Z</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Sandoz B.V._x000d_
+Veluwezoom 22_x000d_
+1327 AH Almere_x000d_
+Netherlands</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>DASATINIB null 70 mg</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>L01XE06 dasatinib</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (AT),Dasatinib Sandoz 70 mg filmomhulde tabletten (BE),Dasatinib Sandoz (CZ),Dasatinib PharOS 70 mg Filmtabletten (DE),Dasatinib "Sandoz" (DK), (EE), (FI), (FR), (HR),DASATINIB SANDOZ  70 mg filmtabletta (HU), (IT),Dasatinib Sandoz 70 mgplėvele dengtos tabletės (LT),Dasatinib Sandoz 70 mg apvalkotās tabletes (LV), (NO),Dasatinib Sandoz 70 mg comprimate filmate (RO), (SE),Dasatinib Sandoz 70 mg filmsko obložene tablete (SI),Dasatinib PharOS 70 mg (SK), (XI)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Film-coated tablet</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='8dce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='c0cf537d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e746d581-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e846d581-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Abridged</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Additional Strength/Form</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Chemical Substance</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Prescription Only</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>NL/H/4002/005</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4002/005</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>DasatinibSandoz 100 mg, filmomhulde tabletten</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2018-07-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2023-01-20T11:02:09.54Z</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Sandoz B.V._x000d_
+Veluwezoom 22_x000d_
+1327 AH Almere_x000d_
+Netherlands</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>DASATINIB null 100 mg</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>L01XE06 dasatinib</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (AT),Dasatinib Sandoz 100 mg filmomhulde tabletten (BE),Dastinib PharOS (BG),Dasatinib PharOS 100 mg Filmtabletten (DE),Dasatinib "Sandoz" (DK), (EE), (FR), (HR),DASATINIB SANDOZ 100 mg filmtabletta (HU), (IT),Dasatinib Sandoz 100 mg plėvele dengtos tabletės (LT),Dasatinib Sandoz 100 mg apvalkotās tabletes (LV),Dasatinib Sandoz (PL), (PT),Dasatinib Sandoz 100 mg comprimate filmate (RO), (SE),Dasatinib Sandoz 100 mg filmsko obložene tablete (SI), (SK), (XI)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Film-coated tablet</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='95ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='becf537d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='eb46d581-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='ec46d581-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Abridged</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Additional Strength/Form</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Chemical Substance</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Prescription Only</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NL/H/4003/006</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4003/006</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dasatinib CF 140 mg, filmomhulde tabletten</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2018-07-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2023-01-16T12:55:55.737Z</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Centrafarm B.V._x000d_
+Nieuwe Donk 3_x000d_
+4879 AC Etten-Leur_x000d_
+The Netherlands</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>DASATINIB null 140 mg</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>L01XE06 dasatinib</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Dasatinib EG 140 mg filmomhulde tabletten (BE),Becalar 140 mg Filmtabletten (DE), (DK), (FI), (FR),DASATINIB STADA  140 mg filmtabletta (HU), (IS), (IT), (LU),Dasatinib STADA (PL), (SE), (XI)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Film-coated tablet</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='adce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='19ef597d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bd9c457d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='be9c457d-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Abridged</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Additional Strength/Form</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Chemical Substance</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Prescription Only</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NL/H/4002/001</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4002/001</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Dasatinib Sandoz 20 mg, filmomhulde tabletten</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2018-07-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2023-01-20T11:01:38.07Z</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Sandoz B.V._x000d_
+Veluwezoom 22_x000d_
+1327 AH Almere_x000d_
+Netherlands</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>DASATINIB null 20 mg</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>L01XE06 dasatinib</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (AT),Dasatinib Sandoz 20 mg filmomhulde tabletten (BE),Dasatinib PharOS (BG),Dasatinib Sandoz (CZ),Dasatinib PharOS 20 mg Filmtabletten (DE),Dasatinib "Sandoz" (DK), (EE), (FI), (FR), (HR),DASATINIB SANDOZ  20 mg filmtabletta (HU), (IT),Dasatinib Sandoz 20 mg plėvele dengtos tabletės (LT),Dasatinib Sandoz 20 mg apvalkotās tabletes (LV), (NO),Dasatinib Sandoz (PL), (PT),Dasatinib Sandoz 20 mg comprimate filmate (RO), (SE),Dasatinib Sandoz 20 mg filmsko obložene tablete (SI),Dasatinib PharOS 20 mg (SK), (XI)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Film-coated tablet</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='89ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bbcf537d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e346d581-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e446d581-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Abridged</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Multiple (Copy) Application</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Chemical Substance</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Prescription Only</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NL/H/4003/005</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4003/005</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Dasatinib CF 100 mg, filmomhulde tabletten</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2018-07-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2023-01-16T12:55:54.923Z</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Centrafarm B.V._x000d_
+Nieuwe Donk 3_x000d_
+4879 AC Etten-Leur_x000d_
+The Netherlands</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>DASATINIB null 100 mg</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>L01XE06 dasatinib</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Dasatinib EG 100 mg filmomhulde tabletten (BE),Becalar 100 mg Filmtabletten (DE), (DK), (FI), (FR), (HR),DASATINIB STADA  100 mg filmtabletta (HU), (IE), (IS), (IT), (LU),Dasatinib STADA (PL),Dasatinib STADA 100 mg comprimate filmate (RO), (SE), (XI)</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Film-coated tablet</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='abce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='1aef597d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bb9c457d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bc9c457d-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Abridged</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Additional Strength/Form</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Chemical Substance</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Prescription Only</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>NL/H/4003/004</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4003/004</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Dasatinib CF 80 mg, filmomhulde tabletten</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2018-07-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2023-01-16T12:55:53.86Z</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Centrafarm B.V._x000d_
+Nieuwe Donk 3_x000d_
+4879 AC Etten-Leur_x000d_
+The Netherlands</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>DASATINIB null 80 mg</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>L01XE06 dasatinib</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Dasatinib EG 80 mg filmomhulde tabletten (BE),Becalar 80 mg Filmtabletten (DE), (DK), (FI),DASATINIB STADA  80 mg filmtabletta (HU), (IS), (IT), (LU),Dasatinib STADA (PL), (SE), (XI)</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Film-coated tablet</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='a6ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='1bef597d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='b99c457d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='ba9c457d-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Abridged</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Additional Strength/Form</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Chemical Substance</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Prescription Only</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NL/H/4003/003</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4003/003</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Dasatinib CF 70 mg, filmomhulde tabletten</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2018-07-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2023-01-16T12:55:53.063Z</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Centrafarm B.V._x000d_
+Nieuwe Donk 3_x000d_
+4879 AC Etten-Leur_x000d_
+The Netherlands</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>DASATINIB null 70 mg</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>L01XE06 dasatinib</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Dasatinib EG 70 mg filmomhulde tabletten (BE),Becalar 70 mg Filmtabletten (DE), (DK), (FI), (FR),DASATINIB STADA  70 mg filmtabletta (HU), (IE), (IS), (IT), (LU),Dasatinib STADA (PL), (SE)</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Film-coated tablet</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='a4ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='1cef597d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='b79c457d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='b89c457d-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Abridged</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Additional Strength/Form</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Chemical Substance</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Prescription Only</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NL/H/4002/002</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4002/002</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Dasatinib Sandoz 50 mg, filmomhulde tabletten</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2018-07-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2023-01-20T11:01:44.96Z</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Sandoz B.V._x000d_
+Veluwezoom 22_x000d_
+1327 AH Almere_x000d_
+Netherlands</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>DASATINIB null 50 mg</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>L01XE06 dasatinib</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (AT),Dasatinib Sandoz 50 mg filmomhulde tabletten (BE),Dasatinib PharOS (BG),Dasatinib Sandoz (CZ),Dasatinib PharOS 50 mg Filmtabletten (DE),Dasatinib "Sandoz" (DK), (EE), (FI), (FR), (HR),DASATINIB SANDOZ  50 mg filmtabletta (HU), (IT),Dasatinib Sandoz 50 mg plėvele dengtos tabletės (LT),Dasatinib Sandoz 50 mg apvalkotās tabletes (LV), (NO),Dasatinib Sandoz (PL), (PT),Dasatinib Sandoz 50 mg comprimate filmate (RO), (SE),Dasatinib Sandoz 50 mg filmsko obložene tablete (SI),Dasatinib PharOS 50 mg (SK), (XI)</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Film-coated tablet</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='8bce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bccf537d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e546d581-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e646d581-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Abridged</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Additional Strength/Form</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Chemical Substance</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Prescription Only</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NL/H/4002/004</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4002/004</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Dasatinib Sandoz 80 mg, filmomhulde tabletten</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2018-07-25T00:00:00Z</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2023-01-20T11:02:13.197Z</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Sandoz B.V._x000d_
+Veluwezoom 22_x000d_
+1327 AH Almere_x000d_
+Netherlands</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>DASATINIB null 80 mg</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>L01XE06 dasatinib</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (AT),Dasatinib PharOS 80 mg Filmtabletten (DE), (EE), (HR), (IT),Dasatinib Sandoz 80 mg plėvele dengtos tabletės (LT),Dasatinib Sandoz 80 mg apvalkotās tabletes (LV),Dasatinib PharOS (PL), (PT), (SE),Dasatinib Sandoz 80 mg filmsko obložene tablete (SI), (XI)</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Film-coated tablet</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='93ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bfcf537d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e946d581-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='ea46d581-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Abridged</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Additional Strength/Form</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Chemical Substance</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Prescription Only</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Down all and final xlsx merged
</commit_message>
<xml_diff>
--- a/res.xlsx
+++ b/res.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,17 +740,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NL/H/4003/006</t>
+          <t>NL/H/4002/004</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4003/006</t>
+          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4002/004</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dasatinib CF 140 mg, filmomhulde tabletten</t>
+          <t>Dasatinib Sandoz 80 mg, filmomhulde tabletten</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -770,111 +770,10 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2023-01-16T12:55:55.737Z</t>
+          <t>2023-01-20T11:02:13.197Z</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
-        <is>
-          <t>Centrafarm B.V._x000d_
-Nieuwe Donk 3_x000d_
-4879 AC Etten-Leur_x000d_
-The Netherlands</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>DASATINIB null 140 mg</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>L01XE06 dasatinib</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Dasatinib EG 140 mg filmomhulde tabletten (BE),Becalar 140 mg Filmtabletten (DE), (DK), (FI), (FR),DASATINIB STADA  140 mg filmtabletta (HU), (IS), (IT), (LU),Dasatinib STADA (PL), (SE), (XI)</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Film-coated tablet</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='adce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='19ef597d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bd9c457d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='be9c457d-da29-eb11-80eb-0050569c593a')/Download</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Abridged</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Additional Strength/Form</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Chemical Substance</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Prescription Only</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>NL/H/4002/001</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4002/001</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Dasatinib Sandoz 20 mg, filmomhulde tabletten</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2018-07-25T00:00:00Z</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2023-01-20T11:01:38.07Z</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Sandoz B.V._x000d_
 Veluwezoom 22_x000d_
@@ -882,563 +781,58 @@
 Netherlands</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Netherlands</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>DASATINIB null 20 mg</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>DASATINIB null 80 mg</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>L01XE06 dasatinib</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (AT),Dasatinib Sandoz 20 mg filmomhulde tabletten (BE),Dasatinib PharOS (BG),Dasatinib Sandoz (CZ),Dasatinib PharOS 20 mg Filmtabletten (DE),Dasatinib "Sandoz" (DK), (EE), (FI), (FR), (HR),DASATINIB SANDOZ  20 mg filmtabletta (HU), (IT),Dasatinib Sandoz 20 mg plėvele dengtos tabletės (LT),Dasatinib Sandoz 20 mg apvalkotās tabletes (LV), (NO),Dasatinib Sandoz (PL), (PT),Dasatinib Sandoz 20 mg comprimate filmate (RO), (SE),Dasatinib Sandoz 20 mg filmsko obložene tablete (SI),Dasatinib PharOS 20 mg (SK), (XI)</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
+      <c r="L4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (AT),Dasatinib PharOS 80 mg Filmtabletten (DE), (EE), (HR), (IT),Dasatinib Sandoz 80 mg plėvele dengtos tabletės (LT),Dasatinib Sandoz 80 mg apvalkotās tabletes (LV),Dasatinib PharOS (PL), (PT), (SE),Dasatinib Sandoz 80 mg filmsko obložene tablete (SI), (XI)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>Film-coated tablet</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='89ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bbcf537d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e346d581-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e446d581-da29-eb11-80eb-0050569c593a')/Download</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr">
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='93ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bfcf537d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e946d581-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='ea46d581-da29-eb11-80eb-0050569c593a')/Download</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
         <is>
           <t>Abridged</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Multiple (Copy) Application</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Additional Strength/Form</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
         <is>
           <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>Chemical Substance</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Prescription Only</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>NL/H/4003/005</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4003/005</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Dasatinib CF 100 mg, filmomhulde tabletten</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2018-07-25T00:00:00Z</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2023-01-16T12:55:54.923Z</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Centrafarm B.V._x000d_
-Nieuwe Donk 3_x000d_
-4879 AC Etten-Leur_x000d_
-The Netherlands</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>DASATINIB null 100 mg</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>L01XE06 dasatinib</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Dasatinib EG 100 mg filmomhulde tabletten (BE),Becalar 100 mg Filmtabletten (DE), (DK), (FI), (FR), (HR),DASATINIB STADA  100 mg filmtabletta (HU), (IE), (IS), (IT), (LU),Dasatinib STADA (PL),Dasatinib STADA 100 mg comprimate filmate (RO), (SE), (XI)</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Film-coated tablet</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='abce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='1aef597d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bb9c457d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bc9c457d-da29-eb11-80eb-0050569c593a')/Download</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Abridged</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>Additional Strength/Form</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>Chemical Substance</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>Prescription Only</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>NL/H/4003/004</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4003/004</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Dasatinib CF 80 mg, filmomhulde tabletten</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2018-07-25T00:00:00Z</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2023-01-16T12:55:53.86Z</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Centrafarm B.V._x000d_
-Nieuwe Donk 3_x000d_
-4879 AC Etten-Leur_x000d_
-The Netherlands</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>DASATINIB null 80 mg</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>L01XE06 dasatinib</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Dasatinib EG 80 mg filmomhulde tabletten (BE),Becalar 80 mg Filmtabletten (DE), (DK), (FI),DASATINIB STADA  80 mg filmtabletta (HU), (IS), (IT), (LU),Dasatinib STADA (PL), (SE), (XI)</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Film-coated tablet</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='a6ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='1bef597d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='b99c457d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='ba9c457d-da29-eb11-80eb-0050569c593a')/Download</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>Abridged</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>Additional Strength/Form</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>Chemical Substance</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>Prescription Only</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>NL/H/4003/003</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4003/003</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Dasatinib CF 70 mg, filmomhulde tabletten</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2018-07-25T00:00:00Z</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2023-01-16T12:55:53.063Z</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Centrafarm B.V._x000d_
-Nieuwe Donk 3_x000d_
-4879 AC Etten-Leur_x000d_
-The Netherlands</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>DASATINIB null 70 mg</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>L01XE06 dasatinib</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Dasatinib EG 70 mg filmomhulde tabletten (BE),Becalar 70 mg Filmtabletten (DE), (DK), (FI), (FR),DASATINIB STADA  70 mg filmtabletta (HU), (IE), (IS), (IT), (LU),Dasatinib STADA (PL), (SE)</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Film-coated tablet</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='a4ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='1cef597d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='b79c457d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='b89c457d-da29-eb11-80eb-0050569c593a')/Download</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Abridged</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Additional Strength/Form</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>Chemical Substance</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>Prescription Only</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>NL/H/4002/002</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4002/002</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Dasatinib Sandoz 50 mg, filmomhulde tabletten</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2018-07-25T00:00:00Z</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2023-01-20T11:01:44.96Z</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Sandoz B.V._x000d_
-Veluwezoom 22_x000d_
-1327 AH Almere_x000d_
-Netherlands</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>DASATINIB null 50 mg</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>L01XE06 dasatinib</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (AT),Dasatinib Sandoz 50 mg filmomhulde tabletten (BE),Dasatinib PharOS (BG),Dasatinib Sandoz (CZ),Dasatinib PharOS 50 mg Filmtabletten (DE),Dasatinib "Sandoz" (DK), (EE), (FI), (FR), (HR),DASATINIB SANDOZ  50 mg filmtabletta (HU), (IT),Dasatinib Sandoz 50 mg plėvele dengtos tabletės (LT),Dasatinib Sandoz 50 mg apvalkotās tabletes (LV), (NO),Dasatinib Sandoz (PL), (PT),Dasatinib Sandoz 50 mg comprimate filmate (RO), (SE),Dasatinib Sandoz 50 mg filmsko obložene tablete (SI),Dasatinib PharOS 50 mg (SK), (XI)</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Film-coated tablet</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='8bce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bccf537d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e546d581-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e646d581-da29-eb11-80eb-0050569c593a')/Download</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Abridged</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Additional Strength/Form</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>Chemical Substance</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>Prescription Only</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>NL/H/4002/004</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/details?productnumber=NL/H/4002/004</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Dasatinib Sandoz 80 mg, filmomhulde tabletten</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2018-07-25T00:00:00Z</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2023-01-20T11:02:13.197Z</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Sandoz B.V._x000d_
-Veluwezoom 22_x000d_
-1327 AH Almere_x000d_
-Netherlands</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>DASATINIB null 80 mg</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>L01XE06 dasatinib</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (AT),Dasatinib PharOS 80 mg Filmtabletten (DE), (EE), (HR), (IT),Dasatinib Sandoz 80 mg plėvele dengtos tabletės (LT),Dasatinib Sandoz 80 mg apvalkotās tabletes (LV),Dasatinib PharOS (PL), (PT), (SE),Dasatinib Sandoz 80 mg filmsko obložene tablete (SI), (XI)</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Film-coated tablet</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='93ce0f7d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='bfcf537d-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='e946d581-da29-eb11-80eb-0050569c593a')/Download | https://mri.cts-mrp.eu/portal/v1/odata/Document(documentApiId='ea46d581-da29-eb11-80eb-0050569c593a')/Download</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>Abridged</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Additional Strength/Form</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Generic Art 10.1 and 10.2 Dir 2001/83/EC</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>Chemical Substance</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>Prescription Only</t>
         </is>

</xml_diff>